<commit_message>
se realizo todas las clases para la otra semana de computacion aplicada 2
</commit_message>
<xml_diff>
--- a/2015-2016/clases/informatica_aplicada/clase_2/listado_alumnos.xlsx
+++ b/2015-2016/clases/informatica_aplicada/clase_2/listado_alumnos.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -418,7 +418,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -533,11 +532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="110525056"/>
-        <c:axId val="110539136"/>
+        <c:axId val="11214848"/>
+        <c:axId val="11216384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="110525056"/>
+        <c:axId val="11214848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110539136"/>
+        <c:crossAx val="11216384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -554,7 +553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="110539136"/>
+        <c:axId val="11216384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,14 +564,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="110525056"/>
+        <c:crossAx val="11214848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1073,7 +1071,7 @@
   <dimension ref="A2:O1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1615,7 @@
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
-        <f t="shared" ref="C21:C31" si="3">C6</f>
+        <f t="shared" ref="C21:C30" si="3">C6</f>
         <v>Alan Ramon</v>
       </c>
       <c r="D21">
@@ -1648,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="24">
-        <f t="shared" ref="F21:F30" si="5">E22*11/100</f>
+        <f t="shared" ref="F22:F30" si="5">E22*11/100</f>
         <v>0.22</v>
       </c>
       <c r="H22" s="12">

</xml_diff>

<commit_message>
se termino bien los syllabus
</commit_message>
<xml_diff>
--- a/2015-2016/clases/informatica_aplicada/clase_2/listado_alumnos.xlsx
+++ b/2015-2016/clases/informatica_aplicada/clase_2/listado_alumnos.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -418,6 +418,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -532,11 +533,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="11214848"/>
-        <c:axId val="11216384"/>
+        <c:axId val="141899648"/>
+        <c:axId val="118321536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11214848"/>
+        <c:axId val="141899648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -545,7 +546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11216384"/>
+        <c:crossAx val="118321536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -553,7 +554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11216384"/>
+        <c:axId val="118321536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -564,13 +565,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="11214848"/>
+        <c:crossAx val="141899648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1070,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>